<commit_message>
working on huge assigment finally
</commit_message>
<xml_diff>
--- a/group2 project/exported_real_net_to_excel.xlsx
+++ b/group2 project/exported_real_net_to_excel.xlsx
@@ -2600,10 +2600,10 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>55</v>
+        <v>53.9</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>10.94486180817282</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2632,10 +2632,10 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>29.84962311319861</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2664,10 +2664,10 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>55</v>
+        <v>53.9</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10.94486180817282</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -2696,10 +2696,10 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>55</v>
+        <v>53.9</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>10.94486180817282</v>
       </c>
       <c r="F5">
         <v>0</v>

</xml_diff>

<commit_message>
añadidas dos lines dobles
</commit_message>
<xml_diff>
--- a/group2 project/exported_real_net_to_excel.xlsx
+++ b/group2 project/exported_real_net_to_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="193">
   <si>
     <t>name</t>
   </si>
@@ -192,6 +192,12 @@
     <t>Line5</t>
   </si>
   <si>
+    <t>Line6</t>
+  </si>
+  <si>
+    <t>Line7</t>
+  </si>
+  <si>
     <t>single</t>
   </si>
   <si>
@@ -249,232 +255,232 @@
     <t>tap_phase_shifter</t>
   </si>
   <si>
+    <t>200MVA</t>
+  </si>
+  <si>
+    <t>hv</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>coords</t>
+  </si>
+  <si>
+    <t>q_mm2</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>NAYY 4x50 SE</t>
+  </si>
+  <si>
+    <t>NAYY 4x120 SE</t>
+  </si>
+  <si>
+    <t>NAYY 4x150 SE</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x95 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x185 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x240 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x95 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x185 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x240 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x150 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x120 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x70 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x150 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x120 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x70 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x120 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x185 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x240 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x300 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>15-AL1/3-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>24-AL1/4-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>34-AL1/6-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>70-AL1/11-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>122-AL1/20-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>149-AL1/24-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>34-AL1/6-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>70-AL1/11-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>122-AL1/20-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>149-AL1/24-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>184-AL1/30-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>243-AL1/39-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>70-AL1/11-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>122-AL1/20-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>149-AL1/24-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>184-AL1/30-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>243-AL1/39-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>305-AL1/39-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>490-AL1/64-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>679-AL1/86-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>490-AL1/64-ST1A 220.0</t>
+  </si>
+  <si>
+    <t>679-AL1/86-ST1A 220.0</t>
+  </si>
+  <si>
+    <t>490-AL1/64-ST1A 380.0</t>
+  </si>
+  <si>
+    <t>679-AL1/86-ST1A 380.0</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>ol</t>
+  </si>
+  <si>
+    <t>vector_group</t>
+  </si>
+  <si>
+    <t>160 MVA 380/110 kV</t>
+  </si>
+  <si>
+    <t>100 MVA 220/110 kV</t>
+  </si>
+  <si>
+    <t>63 MVA 110/20 kV</t>
+  </si>
+  <si>
+    <t>40 MVA 110/20 kV</t>
+  </si>
+  <si>
+    <t>25 MVA 110/20 kV</t>
+  </si>
+  <si>
+    <t>63 MVA 110/10 kV</t>
+  </si>
+  <si>
+    <t>40 MVA 110/10 kV</t>
+  </si>
+  <si>
+    <t>25 MVA 110/10 kV</t>
+  </si>
+  <si>
+    <t>0.25 MVA 20/0.4 kV</t>
+  </si>
+  <si>
+    <t>0.4 MVA 20/0.4 kV</t>
+  </si>
+  <si>
+    <t>0.63 MVA 20/0.4 kV</t>
+  </si>
+  <si>
+    <t>0.25 MVA 10/0.4 kV</t>
+  </si>
+  <si>
+    <t>0.4 MVA 10/0.4 kV</t>
+  </si>
+  <si>
+    <t>0.63 MVA 10/0.4 kV</t>
+  </si>
+  <si>
     <t>100MVA</t>
-  </si>
-  <si>
-    <t>200MVA</t>
-  </si>
-  <si>
-    <t>hv</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>coords</t>
-  </si>
-  <si>
-    <t>q_mm2</t>
-  </si>
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
-    <t>NAYY 4x50 SE</t>
-  </si>
-  <si>
-    <t>NAYY 4x120 SE</t>
-  </si>
-  <si>
-    <t>NAYY 4x150 SE</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x95 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x185 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x240 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x95 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x185 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x240 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x150 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x120 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x70 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x150 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x120 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x70 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x120 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x185 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x240 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x300 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>15-AL1/3-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>24-AL1/4-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>34-AL1/6-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>70-AL1/11-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>122-AL1/20-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>149-AL1/24-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>34-AL1/6-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>70-AL1/11-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>122-AL1/20-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>149-AL1/24-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>184-AL1/30-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>243-AL1/39-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>70-AL1/11-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>122-AL1/20-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>149-AL1/24-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>184-AL1/30-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>243-AL1/39-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>305-AL1/39-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>490-AL1/64-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>679-AL1/86-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>490-AL1/64-ST1A 220.0</t>
-  </si>
-  <si>
-    <t>679-AL1/86-ST1A 220.0</t>
-  </si>
-  <si>
-    <t>490-AL1/64-ST1A 380.0</t>
-  </si>
-  <si>
-    <t>679-AL1/86-ST1A 380.0</t>
-  </si>
-  <si>
-    <t>cs</t>
-  </si>
-  <si>
-    <t>ol</t>
-  </si>
-  <si>
-    <t>vector_group</t>
-  </si>
-  <si>
-    <t>160 MVA 380/110 kV</t>
-  </si>
-  <si>
-    <t>100 MVA 220/110 kV</t>
-  </si>
-  <si>
-    <t>63 MVA 110/20 kV</t>
-  </si>
-  <si>
-    <t>40 MVA 110/20 kV</t>
-  </si>
-  <si>
-    <t>25 MVA 110/20 kV</t>
-  </si>
-  <si>
-    <t>63 MVA 110/10 kV</t>
-  </si>
-  <si>
-    <t>40 MVA 110/10 kV</t>
-  </si>
-  <si>
-    <t>25 MVA 110/10 kV</t>
-  </si>
-  <si>
-    <t>0.25 MVA 20/0.4 kV</t>
-  </si>
-  <si>
-    <t>0.4 MVA 20/0.4 kV</t>
-  </si>
-  <si>
-    <t>0.63 MVA 20/0.4 kV</t>
-  </si>
-  <si>
-    <t>0.25 MVA 10/0.4 kV</t>
-  </si>
-  <si>
-    <t>0.4 MVA 10/0.4 kV</t>
-  </si>
-  <si>
-    <t>0.63 MVA 10/0.4 kV</t>
   </si>
   <si>
     <t>Yy0</t>
@@ -1231,75 +1237,75 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B2">
         <v>63</v>
@@ -1350,10 +1356,10 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="S2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -1370,7 +1376,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B3">
         <v>63</v>
@@ -1421,10 +1427,10 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="S3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -1454,13 +1460,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1474,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1488,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1502,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1516,7 +1522,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1530,7 +1536,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1538,13 +1544,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1552,13 +1558,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1566,13 +1572,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1580,13 +1586,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1594,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1608,13 +1614,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1622,13 +1628,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1636,13 +1642,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1650,13 +1656,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1664,13 +1670,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1678,13 +1684,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1692,13 +1698,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1706,13 +1712,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1720,13 +1726,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1734,13 +1740,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1748,13 +1754,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1762,13 +1768,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1776,13 +1782,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1790,13 +1796,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1804,13 +1810,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1818,13 +1824,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1832,13 +1838,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1846,13 +1852,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1860,13 +1866,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1874,13 +1880,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1888,13 +1894,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1902,13 +1908,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1916,13 +1922,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1930,13 +1936,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1944,13 +1950,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1958,13 +1964,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C37" t="s">
         <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1972,13 +1978,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
         <v>40</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1986,13 +1992,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C39" t="s">
         <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2000,13 +2006,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
       </c>
       <c r="D40" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2014,13 +2020,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C41" t="s">
         <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2028,13 +2034,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2042,13 +2048,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C43" t="s">
         <v>45</v>
       </c>
       <c r="D43" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2056,13 +2062,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s">
         <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2070,13 +2076,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s">
         <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2084,13 +2090,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
       </c>
       <c r="D46" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2098,13 +2104,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2112,13 +2118,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2126,13 +2132,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2140,13 +2146,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2154,13 +2160,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2168,13 +2174,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2182,13 +2188,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C53" t="s">
         <v>25</v>
       </c>
       <c r="D53" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2196,13 +2202,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2210,13 +2216,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2224,13 +2230,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2238,13 +2244,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D57" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2252,13 +2258,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2266,13 +2272,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2280,13 +2286,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2294,13 +2300,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2308,13 +2314,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2322,13 +2328,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2336,13 +2342,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2350,13 +2356,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D65" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2364,13 +2370,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D66" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2378,13 +2384,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D67" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2392,13 +2398,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C68" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D68" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2406,13 +2412,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C69" t="s">
         <v>48</v>
       </c>
       <c r="D69" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2420,13 +2426,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C70" t="s">
         <v>47</v>
       </c>
       <c r="D70" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2434,13 +2440,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2448,13 +2454,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C72" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D72" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2462,13 +2468,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D73" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2476,13 +2482,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D74" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2500,22 +2506,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>25</v>
@@ -2526,10 +2532,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -2854,7 +2860,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2912,7 +2918,7 @@
         <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2956,7 +2962,7 @@
         <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3000,7 +3006,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3044,7 +3050,7 @@
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -3088,7 +3094,7 @@
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -3132,7 +3138,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3165,6 +3171,94 @@
         <v>1</v>
       </c>
       <c r="O7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>136</v>
+      </c>
+      <c r="G8">
+        <v>0.031</v>
+      </c>
+      <c r="H8">
+        <v>0.191</v>
+      </c>
+      <c r="I8">
+        <v>18.8904</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1.778</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>154</v>
+      </c>
+      <c r="G9">
+        <v>0.031</v>
+      </c>
+      <c r="H9">
+        <v>0.191</v>
+      </c>
+      <c r="I9">
+        <v>18.8904</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1.778</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3189,58 +3283,58 @@
         <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>48</v>
@@ -3257,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3266,7 +3360,7 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G2">
         <v>110</v>
@@ -3275,22 +3369,22 @@
         <v>20</v>
       </c>
       <c r="I2">
-        <v>18</v>
+        <v>12.2</v>
       </c>
       <c r="J2">
-        <v>0.38</v>
+        <v>0.26</v>
       </c>
       <c r="K2">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="L2">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M2">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -3328,7 +3422,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3361,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -3399,7 +3493,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -3408,7 +3502,7 @@
         <v>12</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G4">
         <v>110</v>
@@ -3417,22 +3511,22 @@
         <v>20</v>
       </c>
       <c r="I4">
-        <v>18</v>
+        <v>12.2</v>
       </c>
       <c r="J4">
-        <v>0.38</v>
+        <v>0.26</v>
       </c>
       <c r="K4">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="L4">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M4">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -3470,7 +3564,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -3479,7 +3573,7 @@
         <v>13</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G5">
         <v>110</v>
@@ -3488,22 +3582,22 @@
         <v>20</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>12.2</v>
       </c>
       <c r="J5">
-        <v>0.38</v>
+        <v>0.26</v>
       </c>
       <c r="K5">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="L5">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -3551,13 +3645,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3744,15 +3838,15 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2">
         <v>210</v>
@@ -3767,7 +3861,7 @@
         <v>0.142</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G2">
         <v>50</v>
@@ -3778,7 +3872,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>264</v>
@@ -3793,7 +3887,7 @@
         <v>0.242</v>
       </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G3">
         <v>120</v>
@@ -3804,7 +3898,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>261</v>
@@ -3819,7 +3913,7 @@
         <v>0.27</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -3830,7 +3924,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B5">
         <v>216</v>
@@ -3845,7 +3939,7 @@
         <v>0.252</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G5">
         <v>95</v>
@@ -3856,7 +3950,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B6">
         <v>273</v>
@@ -3871,7 +3965,7 @@
         <v>0.362</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G6">
         <v>185</v>
@@ -3882,7 +3976,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B7">
         <v>304</v>
@@ -3897,7 +3991,7 @@
         <v>0.421</v>
       </c>
       <c r="F7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G7">
         <v>240</v>
@@ -3908,7 +4002,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>315</v>
@@ -3923,7 +4017,7 @@
         <v>0.249</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G8">
         <v>95</v>
@@ -3934,7 +4028,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B9">
         <v>406</v>
@@ -3949,7 +4043,7 @@
         <v>0.358</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G9">
         <v>185</v>
@@ -3960,7 +4054,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>456</v>
@@ -3975,7 +4069,7 @@
         <v>0.416</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G10">
         <v>240</v>
@@ -3986,7 +4080,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B11">
         <v>250</v>
@@ -4001,7 +4095,7 @@
         <v>0.319</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G11">
         <v>150</v>
@@ -4012,7 +4106,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B12">
         <v>230</v>
@@ -4027,7 +4121,7 @@
         <v>0.283</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G12">
         <v>120</v>
@@ -4038,7 +4132,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B13">
         <v>190</v>
@@ -4053,7 +4147,7 @@
         <v>0.22</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G13">
         <v>70</v>
@@ -4064,7 +4158,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B14">
         <v>360</v>
@@ -4079,7 +4173,7 @@
         <v>0.315</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G14">
         <v>150</v>
@@ -4090,7 +4184,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B15">
         <v>340</v>
@@ -4105,7 +4199,7 @@
         <v>0.28</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G15">
         <v>120</v>
@@ -4116,7 +4210,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B16">
         <v>280</v>
@@ -4131,7 +4225,7 @@
         <v>0.217</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G16">
         <v>70</v>
@@ -4142,7 +4236,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B17">
         <v>112</v>
@@ -4157,7 +4251,7 @@
         <v>0.366</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G17">
         <v>120</v>
@@ -4168,7 +4262,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B18">
         <v>125</v>
@@ -4183,7 +4277,7 @@
         <v>0.457</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G18">
         <v>185</v>
@@ -4194,7 +4288,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>135</v>
@@ -4209,7 +4303,7 @@
         <v>0.526</v>
       </c>
       <c r="F19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G19">
         <v>240</v>
@@ -4220,7 +4314,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20">
         <v>144</v>
@@ -4235,7 +4329,7 @@
         <v>0.588</v>
       </c>
       <c r="F20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G20">
         <v>300</v>
@@ -4246,7 +4340,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -4261,7 +4355,7 @@
         <v>0.105</v>
       </c>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G21">
         <v>16</v>
@@ -4272,7 +4366,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B22">
         <v>11.25</v>
@@ -4287,7 +4381,7 @@
         <v>0.14</v>
       </c>
       <c r="F22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G22">
         <v>24</v>
@@ -4298,7 +4392,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B23">
         <v>12.2</v>
@@ -4313,7 +4407,7 @@
         <v>0.21</v>
       </c>
       <c r="F23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G23">
         <v>48</v>
@@ -4324,7 +4418,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B24">
         <v>13.2</v>
@@ -4339,7 +4433,7 @@
         <v>0.35</v>
       </c>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G24">
         <v>94</v>
@@ -4350,7 +4444,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B25">
         <v>9.699999999999999</v>
@@ -4365,7 +4459,7 @@
         <v>0.17</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G25">
         <v>34</v>
@@ -4376,7 +4470,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B26">
         <v>10.1</v>
@@ -4391,7 +4485,7 @@
         <v>0.21</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G26">
         <v>48</v>
@@ -4402,7 +4496,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B27">
         <v>10.4</v>
@@ -4417,7 +4511,7 @@
         <v>0.29</v>
       </c>
       <c r="F27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G27">
         <v>70</v>
@@ -4428,7 +4522,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B28">
         <v>10.75</v>
@@ -4443,7 +4537,7 @@
         <v>0.35</v>
       </c>
       <c r="F28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G28">
         <v>94</v>
@@ -4454,7 +4548,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B29">
         <v>11.1</v>
@@ -4469,7 +4563,7 @@
         <v>0.41</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G29">
         <v>122</v>
@@ -4480,7 +4574,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B30">
         <v>11.25</v>
@@ -4495,7 +4589,7 @@
         <v>0.47</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G30">
         <v>149</v>
@@ -4506,7 +4600,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B31">
         <v>9.15</v>
@@ -4521,7 +4615,7 @@
         <v>0.17</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G31">
         <v>34</v>
@@ -4532,7 +4626,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B32">
         <v>9.5</v>
@@ -4547,7 +4641,7 @@
         <v>0.21</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G32">
         <v>48</v>
@@ -4558,7 +4652,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B33">
         <v>9.699999999999999</v>
@@ -4573,7 +4667,7 @@
         <v>0.29</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G33">
         <v>70</v>
@@ -4584,7 +4678,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -4599,7 +4693,7 @@
         <v>0.35</v>
       </c>
       <c r="F34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G34">
         <v>94</v>
@@ -4610,7 +4704,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B35">
         <v>10.3</v>
@@ -4625,7 +4719,7 @@
         <v>0.41</v>
       </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G35">
         <v>122</v>
@@ -4636,7 +4730,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B36">
         <v>10.5</v>
@@ -4651,7 +4745,7 @@
         <v>0.47</v>
       </c>
       <c r="F36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G36">
         <v>149</v>
@@ -4662,7 +4756,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B37">
         <v>10.75</v>
@@ -4677,7 +4771,7 @@
         <v>0.535</v>
       </c>
       <c r="F37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G37">
         <v>184</v>
@@ -4688,7 +4782,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B38">
         <v>11</v>
@@ -4703,7 +4797,7 @@
         <v>0.645</v>
       </c>
       <c r="F38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G38">
         <v>243</v>
@@ -4714,7 +4808,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -4729,7 +4823,7 @@
         <v>0.21</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G39">
         <v>48</v>
@@ -4740,7 +4834,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B40">
         <v>8.4</v>
@@ -4755,7 +4849,7 @@
         <v>0.29</v>
       </c>
       <c r="F40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G40">
         <v>70</v>
@@ -4766,7 +4860,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B41">
         <v>8.65</v>
@@ -4781,7 +4875,7 @@
         <v>0.35</v>
       </c>
       <c r="F41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G41">
         <v>94</v>
@@ -4792,7 +4886,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B42">
         <v>8.5</v>
@@ -4807,7 +4901,7 @@
         <v>0.41</v>
       </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42">
         <v>122</v>
@@ -4818,7 +4912,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B43">
         <v>8.75</v>
@@ -4833,7 +4927,7 @@
         <v>0.47</v>
       </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G43">
         <v>149</v>
@@ -4844,7 +4938,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B44">
         <v>8.800000000000001</v>
@@ -4859,7 +4953,7 @@
         <v>0.535</v>
       </c>
       <c r="F44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G44">
         <v>184</v>
@@ -4870,7 +4964,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B45">
         <v>9</v>
@@ -4885,7 +4979,7 @@
         <v>0.645</v>
       </c>
       <c r="F45" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G45">
         <v>243</v>
@@ -4896,7 +4990,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B46">
         <v>9.199999999999999</v>
@@ -4911,7 +5005,7 @@
         <v>0.74</v>
       </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G46">
         <v>305</v>
@@ -4922,7 +5016,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B47">
         <v>9.75</v>
@@ -4937,7 +5031,7 @@
         <v>0.96</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G47">
         <v>490</v>
@@ -4948,7 +5042,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B48">
         <v>9.949999999999999</v>
@@ -4963,7 +5057,7 @@
         <v>1.15</v>
       </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G48">
         <v>679</v>
@@ -4974,7 +5068,7 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B49">
         <v>10</v>
@@ -4989,7 +5083,7 @@
         <v>0.96</v>
       </c>
       <c r="F49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G49">
         <v>490</v>
@@ -5000,7 +5094,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50">
         <v>11.7</v>
@@ -5015,7 +5109,7 @@
         <v>1.15</v>
       </c>
       <c r="F50" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G50">
         <v>679</v>
@@ -5026,7 +5120,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B51">
         <v>11</v>
@@ -5041,7 +5135,7 @@
         <v>0.96</v>
       </c>
       <c r="F51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G51">
         <v>490</v>
@@ -5052,7 +5146,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B52">
         <v>14.6</v>
@@ -5067,7 +5161,7 @@
         <v>1.15</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G52">
         <v>679</v>
@@ -5078,7 +5172,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B53">
         <v>9.06</v>
@@ -5095,7 +5189,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B54">
         <v>18.8904</v>
@@ -5125,57 +5219,57 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B2">
         <v>0.06</v>
@@ -5202,10 +5296,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -5228,7 +5322,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B3">
         <v>0.06</v>
@@ -5255,10 +5349,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -5281,7 +5375,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>0.04</v>
@@ -5308,10 +5402,10 @@
         <v>150</v>
       </c>
       <c r="J4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5334,7 +5428,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -5361,10 +5455,10 @@
         <v>150</v>
       </c>
       <c r="J5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5387,7 +5481,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B6">
         <v>0.07000000000000001</v>
@@ -5414,10 +5508,10 @@
         <v>150</v>
       </c>
       <c r="J6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -5440,7 +5534,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B7">
         <v>0.04</v>
@@ -5467,10 +5561,10 @@
         <v>150</v>
       </c>
       <c r="J7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5493,7 +5587,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -5520,10 +5614,10 @@
         <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -5546,7 +5640,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B9">
         <v>0.07000000000000001</v>
@@ -5573,10 +5667,10 @@
         <v>150</v>
       </c>
       <c r="J9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -5599,7 +5693,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B10">
         <v>0.32</v>
@@ -5626,10 +5720,10 @@
         <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -5652,7 +5746,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B11">
         <v>0.3375</v>
@@ -5679,10 +5773,10 @@
         <v>150</v>
       </c>
       <c r="J11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -5705,7 +5799,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B12">
         <v>0.2619</v>
@@ -5732,10 +5826,10 @@
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -5758,7 +5852,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B13">
         <v>0.24</v>
@@ -5785,10 +5879,10 @@
         <v>150</v>
       </c>
       <c r="J13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -5811,7 +5905,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B14">
         <v>0.2375</v>
@@ -5838,10 +5932,10 @@
         <v>150</v>
       </c>
       <c r="J14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -5864,7 +5958,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B15">
         <v>0.1873</v>
@@ -5891,10 +5985,10 @@
         <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -5917,7 +6011,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="B16">
         <v>0.04</v>
@@ -5944,10 +6038,10 @@
         <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -5970,7 +6064,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>0.06</v>
@@ -5997,10 +6091,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L17">
         <v>0</v>

</xml_diff>

<commit_message>
fixed issue anthony about Q calculation
</commit_message>
<xml_diff>
--- a/group2 project/exported_real_net_to_excel.xlsx
+++ b/group2 project/exported_real_net_to_excel.xlsx
@@ -2730,7 +2730,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2797,6 +2797,58 @@
         <v>1</v>
       </c>
       <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>17.25</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>42</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
     </row>
@@ -3185,13 +3237,13 @@
         <v>58</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>136</v>
+        <v>15.12</v>
       </c>
       <c r="G8">
         <v>0.031</v>
@@ -3229,13 +3281,13 @@
         <v>58</v>
       </c>
       <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
-        <v>154</v>
+        <v>18.33</v>
       </c>
       <c r="G9">
         <v>0.031</v>

</xml_diff>

<commit_message>
final part, all together
</commit_message>
<xml_diff>
--- a/group2 project/exported_real_net_to_excel.xlsx
+++ b/group2 project/exported_real_net_to_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="200">
   <si>
     <t>name</t>
   </si>
@@ -204,235 +204,250 @@
     <t>Line8</t>
   </si>
   <si>
+    <t>Line9</t>
+  </si>
+  <si>
+    <t>Line10</t>
+  </si>
+  <si>
+    <t>Line11</t>
+  </si>
+  <si>
+    <t>Line12</t>
+  </si>
+  <si>
+    <t>Line13</t>
+  </si>
+  <si>
     <t>single</t>
   </si>
   <si>
+    <t>hv_bus</t>
+  </si>
+  <si>
+    <t>lv_bus</t>
+  </si>
+  <si>
+    <t>vn_hv_kv</t>
+  </si>
+  <si>
+    <t>vn_lv_kv</t>
+  </si>
+  <si>
+    <t>vk_percent</t>
+  </si>
+  <si>
+    <t>vkr_percent</t>
+  </si>
+  <si>
+    <t>pfe_kw</t>
+  </si>
+  <si>
+    <t>i0_percent</t>
+  </si>
+  <si>
+    <t>shift_degree</t>
+  </si>
+  <si>
+    <t>tap_side</t>
+  </si>
+  <si>
+    <t>tap_neutral</t>
+  </si>
+  <si>
+    <t>tap_min</t>
+  </si>
+  <si>
+    <t>tap_max</t>
+  </si>
+  <si>
+    <t>tap_step_percent</t>
+  </si>
+  <si>
+    <t>tap_step_degree</t>
+  </si>
+  <si>
+    <t>tap_pos</t>
+  </si>
+  <si>
+    <t>tap_phase_shifter</t>
+  </si>
+  <si>
+    <t>200MVA</t>
+  </si>
+  <si>
+    <t>hv</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>coords</t>
+  </si>
+  <si>
+    <t>q_mm2</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>NAYY 4x50 SE</t>
+  </si>
+  <si>
+    <t>NAYY 4x120 SE</t>
+  </si>
+  <si>
+    <t>NAYY 4x150 SE</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x95 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x185 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x240 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x95 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x185 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x240 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x150 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x120 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x70 RM/25 12/20 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x150 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x120 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>NA2XS2Y 1x70 RM/25 6/10 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x120 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x185 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x240 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>N2XS(FL)2Y 1x300 RM/35 64/110 kV</t>
+  </si>
+  <si>
+    <t>15-AL1/3-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>24-AL1/4-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 0.4</t>
+  </si>
+  <si>
+    <t>34-AL1/6-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>70-AL1/11-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>122-AL1/20-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>149-AL1/24-ST1A 10.0</t>
+  </si>
+  <si>
+    <t>34-AL1/6-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>70-AL1/11-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>122-AL1/20-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>149-AL1/24-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>184-AL1/30-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>243-AL1/39-ST1A 20.0</t>
+  </si>
+  <si>
+    <t>48-AL1/8-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>70-AL1/11-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>94-AL1/15-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>122-AL1/20-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>149-AL1/24-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>184-AL1/30-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>243-AL1/39-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>305-AL1/39-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>490-AL1/64-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>679-AL1/86-ST1A 110.0</t>
+  </si>
+  <si>
+    <t>490-AL1/64-ST1A 220.0</t>
+  </si>
+  <si>
+    <t>679-AL1/86-ST1A 220.0</t>
+  </si>
+  <si>
+    <t>490-AL1/64-ST1A 380.0</t>
+  </si>
+  <si>
+    <t>679-AL1/86-ST1A 380.0</t>
+  </si>
+  <si>
     <t>double</t>
-  </si>
-  <si>
-    <t>hv_bus</t>
-  </si>
-  <si>
-    <t>lv_bus</t>
-  </si>
-  <si>
-    <t>vn_hv_kv</t>
-  </si>
-  <si>
-    <t>vn_lv_kv</t>
-  </si>
-  <si>
-    <t>vk_percent</t>
-  </si>
-  <si>
-    <t>vkr_percent</t>
-  </si>
-  <si>
-    <t>pfe_kw</t>
-  </si>
-  <si>
-    <t>i0_percent</t>
-  </si>
-  <si>
-    <t>shift_degree</t>
-  </si>
-  <si>
-    <t>tap_side</t>
-  </si>
-  <si>
-    <t>tap_neutral</t>
-  </si>
-  <si>
-    <t>tap_min</t>
-  </si>
-  <si>
-    <t>tap_max</t>
-  </si>
-  <si>
-    <t>tap_step_percent</t>
-  </si>
-  <si>
-    <t>tap_step_degree</t>
-  </si>
-  <si>
-    <t>tap_pos</t>
-  </si>
-  <si>
-    <t>tap_phase_shifter</t>
-  </si>
-  <si>
-    <t>200MVA</t>
-  </si>
-  <si>
-    <t>hv</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>coords</t>
-  </si>
-  <si>
-    <t>q_mm2</t>
-  </si>
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
-    <t>NAYY 4x50 SE</t>
-  </si>
-  <si>
-    <t>NAYY 4x120 SE</t>
-  </si>
-  <si>
-    <t>NAYY 4x150 SE</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x95 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x185 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x240 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x95 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x185 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x240 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x150 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x120 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x70 RM/25 12/20 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x150 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x120 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>NA2XS2Y 1x70 RM/25 6/10 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x120 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x185 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x240 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>N2XS(FL)2Y 1x300 RM/35 64/110 kV</t>
-  </si>
-  <si>
-    <t>15-AL1/3-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>24-AL1/4-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 0.4</t>
-  </si>
-  <si>
-    <t>34-AL1/6-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>70-AL1/11-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>122-AL1/20-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>149-AL1/24-ST1A 10.0</t>
-  </si>
-  <si>
-    <t>34-AL1/6-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>70-AL1/11-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>122-AL1/20-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>149-AL1/24-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>184-AL1/30-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>243-AL1/39-ST1A 20.0</t>
-  </si>
-  <si>
-    <t>48-AL1/8-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>70-AL1/11-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>94-AL1/15-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>122-AL1/20-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>149-AL1/24-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>184-AL1/30-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>243-AL1/39-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>305-AL1/39-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>490-AL1/64-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>679-AL1/86-ST1A 110.0</t>
-  </si>
-  <si>
-    <t>490-AL1/64-ST1A 220.0</t>
-  </si>
-  <si>
-    <t>679-AL1/86-ST1A 220.0</t>
-  </si>
-  <si>
-    <t>490-AL1/64-ST1A 380.0</t>
-  </si>
-  <si>
-    <t>679-AL1/86-ST1A 380.0</t>
   </si>
   <si>
     <t>cs</t>
@@ -1260,75 +1275,75 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B2">
         <v>63</v>
@@ -1379,10 +1394,10 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="S2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -1399,7 +1414,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>63</v>
@@ -1450,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="S3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -1483,13 +1498,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1503,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1517,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1531,7 +1546,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1545,7 +1560,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1559,7 +1574,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1567,13 +1582,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1581,13 +1596,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1595,13 +1610,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1609,13 +1624,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1623,13 +1638,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1637,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1651,13 +1666,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1665,13 +1680,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1679,13 +1694,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1693,13 +1708,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1707,13 +1722,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1721,13 +1736,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1735,13 +1750,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1749,13 +1764,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1763,13 +1778,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1777,13 +1792,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1791,13 +1806,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1805,13 +1820,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1819,13 +1834,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1833,13 +1848,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1847,13 +1862,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1861,13 +1876,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1875,13 +1890,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1889,13 +1904,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C30" t="s">
         <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1903,13 +1918,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1917,13 +1932,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1931,13 +1946,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1945,13 +1960,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1959,13 +1974,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1973,13 +1988,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C36" t="s">
         <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1987,13 +2002,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
         <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2001,13 +2016,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
         <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2015,13 +2030,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
         <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2029,13 +2044,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C40" t="s">
         <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2043,13 +2058,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
         <v>44</v>
       </c>
       <c r="D41" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2057,13 +2072,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2071,13 +2086,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C43" t="s">
         <v>46</v>
       </c>
       <c r="D43" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2085,13 +2100,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C44" t="s">
         <v>47</v>
       </c>
       <c r="D44" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2099,13 +2114,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
         <v>48</v>
       </c>
       <c r="D45" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2113,13 +2128,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C46" t="s">
         <v>49</v>
       </c>
       <c r="D46" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2127,13 +2142,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2141,13 +2156,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2155,13 +2170,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2169,13 +2184,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C50" t="s">
         <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2183,13 +2198,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D51" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2197,13 +2212,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2211,13 +2226,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
       </c>
       <c r="D53" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2225,13 +2240,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2239,13 +2254,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2253,13 +2268,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2267,13 +2282,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2281,13 +2296,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2295,13 +2310,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2309,13 +2324,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D60" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2323,13 +2338,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2337,13 +2352,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2351,13 +2366,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D63" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2365,13 +2380,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2379,13 +2394,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2393,13 +2408,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C66" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D66" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2407,13 +2422,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D67" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2421,13 +2436,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D68" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2435,13 +2450,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C69" t="s">
         <v>49</v>
       </c>
       <c r="D69" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2449,13 +2464,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C70" t="s">
         <v>48</v>
       </c>
       <c r="D70" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2463,13 +2478,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2477,13 +2492,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C72" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D72" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2491,13 +2506,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C73" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D73" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2505,13 +2520,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2529,22 +2544,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>26</v>
@@ -2555,10 +2570,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -2961,7 +2976,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3019,7 +3034,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3063,7 +3078,7 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3075,19 +3090,19 @@
         <v>58</v>
       </c>
       <c r="G3">
-        <v>0.031</v>
+        <v>0.062</v>
       </c>
       <c r="H3">
-        <v>0.191</v>
+        <v>0.398</v>
       </c>
       <c r="I3">
-        <v>18.8904</v>
+        <v>9.06</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>1.778</v>
+        <v>0.889</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3107,7 +3122,7 @@
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3119,19 +3134,19 @@
         <v>30</v>
       </c>
       <c r="G4">
-        <v>0.031</v>
+        <v>0.062</v>
       </c>
       <c r="H4">
-        <v>0.191</v>
+        <v>0.398</v>
       </c>
       <c r="I4">
-        <v>18.8904</v>
+        <v>9.06</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>1.778</v>
+        <v>0.889</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -3151,7 +3166,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -3163,19 +3178,19 @@
         <v>52</v>
       </c>
       <c r="G5">
-        <v>0.031</v>
+        <v>0.062</v>
       </c>
       <c r="H5">
-        <v>0.191</v>
+        <v>0.398</v>
       </c>
       <c r="I5">
-        <v>18.8904</v>
+        <v>9.06</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>1.778</v>
+        <v>0.889</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -3195,7 +3210,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -3239,7 +3254,7 @@
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3283,7 +3298,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -3295,19 +3310,19 @@
         <v>15.12</v>
       </c>
       <c r="G8">
-        <v>0.031</v>
+        <v>0.062</v>
       </c>
       <c r="H8">
-        <v>0.191</v>
+        <v>0.398</v>
       </c>
       <c r="I8">
-        <v>18.8904</v>
+        <v>9.06</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1.778</v>
+        <v>0.889</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -3327,7 +3342,7 @@
         <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -3339,19 +3354,19 @@
         <v>18.33</v>
       </c>
       <c r="G9">
-        <v>0.031</v>
+        <v>0.062</v>
       </c>
       <c r="H9">
-        <v>0.191</v>
+        <v>0.398</v>
       </c>
       <c r="I9">
-        <v>18.8904</v>
+        <v>9.06</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1.778</v>
+        <v>0.889</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -3371,7 +3386,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -3383,19 +3398,19 @@
         <v>11.53</v>
       </c>
       <c r="G10">
-        <v>0.031</v>
+        <v>0.062</v>
       </c>
       <c r="H10">
-        <v>0.191</v>
+        <v>0.398</v>
       </c>
       <c r="I10">
-        <v>18.8904</v>
+        <v>9.06</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1.778</v>
+        <v>0.889</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -3404,6 +3419,270 @@
         <v>1</v>
       </c>
       <c r="O10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>136</v>
+      </c>
+      <c r="G11">
+        <v>0.062</v>
+      </c>
+      <c r="H11">
+        <v>0.398</v>
+      </c>
+      <c r="I11">
+        <v>9.06</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0.889</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>154</v>
+      </c>
+      <c r="G12">
+        <v>0.062</v>
+      </c>
+      <c r="H12">
+        <v>0.398</v>
+      </c>
+      <c r="I12">
+        <v>9.06</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0.889</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>33.44</v>
+      </c>
+      <c r="G13">
+        <v>0.062</v>
+      </c>
+      <c r="H13">
+        <v>0.398</v>
+      </c>
+      <c r="I13">
+        <v>9.06</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.889</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>33.44</v>
+      </c>
+      <c r="G14">
+        <v>0.062</v>
+      </c>
+      <c r="H14">
+        <v>0.398</v>
+      </c>
+      <c r="I14">
+        <v>9.06</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0.889</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>33.44</v>
+      </c>
+      <c r="G15">
+        <v>0.062</v>
+      </c>
+      <c r="H15">
+        <v>0.398</v>
+      </c>
+      <c r="I15">
+        <v>9.06</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0.889</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>33.44</v>
+      </c>
+      <c r="G16">
+        <v>0.062</v>
+      </c>
+      <c r="H16">
+        <v>0.398</v>
+      </c>
+      <c r="I16">
+        <v>9.06</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0.889</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3428,58 +3707,58 @@
         <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>49</v>
@@ -3496,7 +3775,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3529,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -3567,7 +3846,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3600,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -3638,7 +3917,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -3671,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -3709,7 +3988,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -3742,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -3790,13 +4069,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3994,15 +4273,15 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B2">
         <v>210</v>
@@ -4017,7 +4296,7 @@
         <v>0.142</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G2">
         <v>50</v>
@@ -4028,7 +4307,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>264</v>
@@ -4043,7 +4322,7 @@
         <v>0.242</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G3">
         <v>120</v>
@@ -4054,7 +4333,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>261</v>
@@ -4069,7 +4348,7 @@
         <v>0.27</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -4080,7 +4359,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B5">
         <v>216</v>
@@ -4095,7 +4374,7 @@
         <v>0.252</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G5">
         <v>95</v>
@@ -4106,7 +4385,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>273</v>
@@ -4121,7 +4400,7 @@
         <v>0.362</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G6">
         <v>185</v>
@@ -4132,7 +4411,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B7">
         <v>304</v>
@@ -4147,7 +4426,7 @@
         <v>0.421</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G7">
         <v>240</v>
@@ -4158,7 +4437,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>315</v>
@@ -4173,7 +4452,7 @@
         <v>0.249</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G8">
         <v>95</v>
@@ -4184,7 +4463,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <v>406</v>
@@ -4199,7 +4478,7 @@
         <v>0.358</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G9">
         <v>185</v>
@@ -4210,7 +4489,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B10">
         <v>456</v>
@@ -4225,7 +4504,7 @@
         <v>0.416</v>
       </c>
       <c r="F10" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G10">
         <v>240</v>
@@ -4236,7 +4515,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>250</v>
@@ -4251,7 +4530,7 @@
         <v>0.319</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G11">
         <v>150</v>
@@ -4262,7 +4541,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B12">
         <v>230</v>
@@ -4277,7 +4556,7 @@
         <v>0.283</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G12">
         <v>120</v>
@@ -4288,7 +4567,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B13">
         <v>190</v>
@@ -4303,7 +4582,7 @@
         <v>0.22</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G13">
         <v>70</v>
@@ -4314,7 +4593,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <v>360</v>
@@ -4329,7 +4608,7 @@
         <v>0.315</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G14">
         <v>150</v>
@@ -4340,7 +4619,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B15">
         <v>340</v>
@@ -4355,7 +4634,7 @@
         <v>0.28</v>
       </c>
       <c r="F15" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G15">
         <v>120</v>
@@ -4366,7 +4645,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B16">
         <v>280</v>
@@ -4381,7 +4660,7 @@
         <v>0.217</v>
       </c>
       <c r="F16" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G16">
         <v>70</v>
@@ -4392,7 +4671,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B17">
         <v>112</v>
@@ -4407,7 +4686,7 @@
         <v>0.366</v>
       </c>
       <c r="F17" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G17">
         <v>120</v>
@@ -4418,7 +4697,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B18">
         <v>125</v>
@@ -4433,7 +4712,7 @@
         <v>0.457</v>
       </c>
       <c r="F18" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G18">
         <v>185</v>
@@ -4444,7 +4723,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B19">
         <v>135</v>
@@ -4459,7 +4738,7 @@
         <v>0.526</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G19">
         <v>240</v>
@@ -4470,7 +4749,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B20">
         <v>144</v>
@@ -4485,7 +4764,7 @@
         <v>0.588</v>
       </c>
       <c r="F20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G20">
         <v>300</v>
@@ -4496,7 +4775,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -4511,7 +4790,7 @@
         <v>0.105</v>
       </c>
       <c r="F21" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G21">
         <v>16</v>
@@ -4522,7 +4801,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B22">
         <v>11.25</v>
@@ -4537,7 +4816,7 @@
         <v>0.14</v>
       </c>
       <c r="F22" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G22">
         <v>24</v>
@@ -4548,7 +4827,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B23">
         <v>12.2</v>
@@ -4563,7 +4842,7 @@
         <v>0.21</v>
       </c>
       <c r="F23" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G23">
         <v>48</v>
@@ -4574,7 +4853,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B24">
         <v>13.2</v>
@@ -4589,7 +4868,7 @@
         <v>0.35</v>
       </c>
       <c r="F24" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G24">
         <v>94</v>
@@ -4600,7 +4879,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B25">
         <v>9.699999999999999</v>
@@ -4615,7 +4894,7 @@
         <v>0.17</v>
       </c>
       <c r="F25" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G25">
         <v>34</v>
@@ -4626,7 +4905,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B26">
         <v>10.1</v>
@@ -4641,7 +4920,7 @@
         <v>0.21</v>
       </c>
       <c r="F26" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G26">
         <v>48</v>
@@ -4652,7 +4931,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B27">
         <v>10.4</v>
@@ -4667,7 +4946,7 @@
         <v>0.29</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G27">
         <v>70</v>
@@ -4678,7 +4957,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B28">
         <v>10.75</v>
@@ -4693,7 +4972,7 @@
         <v>0.35</v>
       </c>
       <c r="F28" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G28">
         <v>94</v>
@@ -4704,7 +4983,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B29">
         <v>11.1</v>
@@ -4719,7 +4998,7 @@
         <v>0.41</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G29">
         <v>122</v>
@@ -4730,7 +5009,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B30">
         <v>11.25</v>
@@ -4745,7 +5024,7 @@
         <v>0.47</v>
       </c>
       <c r="F30" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G30">
         <v>149</v>
@@ -4756,7 +5035,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B31">
         <v>9.15</v>
@@ -4771,7 +5050,7 @@
         <v>0.17</v>
       </c>
       <c r="F31" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G31">
         <v>34</v>
@@ -4782,7 +5061,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B32">
         <v>9.5</v>
@@ -4797,7 +5076,7 @@
         <v>0.21</v>
       </c>
       <c r="F32" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G32">
         <v>48</v>
@@ -4808,7 +5087,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B33">
         <v>9.699999999999999</v>
@@ -4823,7 +5102,7 @@
         <v>0.29</v>
       </c>
       <c r="F33" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G33">
         <v>70</v>
@@ -4834,7 +5113,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -4849,7 +5128,7 @@
         <v>0.35</v>
       </c>
       <c r="F34" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G34">
         <v>94</v>
@@ -4860,7 +5139,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B35">
         <v>10.3</v>
@@ -4875,7 +5154,7 @@
         <v>0.41</v>
       </c>
       <c r="F35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G35">
         <v>122</v>
@@ -4886,7 +5165,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B36">
         <v>10.5</v>
@@ -4901,7 +5180,7 @@
         <v>0.47</v>
       </c>
       <c r="F36" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G36">
         <v>149</v>
@@ -4912,7 +5191,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B37">
         <v>10.75</v>
@@ -4927,7 +5206,7 @@
         <v>0.535</v>
       </c>
       <c r="F37" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G37">
         <v>184</v>
@@ -4938,7 +5217,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B38">
         <v>11</v>
@@ -4953,7 +5232,7 @@
         <v>0.645</v>
       </c>
       <c r="F38" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G38">
         <v>243</v>
@@ -4964,7 +5243,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -4979,7 +5258,7 @@
         <v>0.21</v>
       </c>
       <c r="F39" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G39">
         <v>48</v>
@@ -4990,7 +5269,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B40">
         <v>8.4</v>
@@ -5005,7 +5284,7 @@
         <v>0.29</v>
       </c>
       <c r="F40" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G40">
         <v>70</v>
@@ -5016,7 +5295,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B41">
         <v>8.65</v>
@@ -5031,7 +5310,7 @@
         <v>0.35</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G41">
         <v>94</v>
@@ -5042,7 +5321,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B42">
         <v>8.5</v>
@@ -5057,7 +5336,7 @@
         <v>0.41</v>
       </c>
       <c r="F42" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G42">
         <v>122</v>
@@ -5068,7 +5347,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B43">
         <v>8.75</v>
@@ -5083,7 +5362,7 @@
         <v>0.47</v>
       </c>
       <c r="F43" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G43">
         <v>149</v>
@@ -5094,7 +5373,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B44">
         <v>8.800000000000001</v>
@@ -5109,7 +5388,7 @@
         <v>0.535</v>
       </c>
       <c r="F44" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G44">
         <v>184</v>
@@ -5120,7 +5399,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B45">
         <v>9</v>
@@ -5135,7 +5414,7 @@
         <v>0.645</v>
       </c>
       <c r="F45" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G45">
         <v>243</v>
@@ -5146,7 +5425,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B46">
         <v>9.199999999999999</v>
@@ -5161,7 +5440,7 @@
         <v>0.74</v>
       </c>
       <c r="F46" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G46">
         <v>305</v>
@@ -5172,7 +5451,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B47">
         <v>9.75</v>
@@ -5187,7 +5466,7 @@
         <v>0.96</v>
       </c>
       <c r="F47" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G47">
         <v>490</v>
@@ -5198,7 +5477,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B48">
         <v>9.949999999999999</v>
@@ -5213,7 +5492,7 @@
         <v>1.15</v>
       </c>
       <c r="F48" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G48">
         <v>679</v>
@@ -5224,7 +5503,7 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B49">
         <v>10</v>
@@ -5239,7 +5518,7 @@
         <v>0.96</v>
       </c>
       <c r="F49" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G49">
         <v>490</v>
@@ -5250,7 +5529,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B50">
         <v>11.7</v>
@@ -5265,7 +5544,7 @@
         <v>1.15</v>
       </c>
       <c r="F50" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G50">
         <v>679</v>
@@ -5276,7 +5555,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B51">
         <v>11</v>
@@ -5291,7 +5570,7 @@
         <v>0.96</v>
       </c>
       <c r="F51" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G51">
         <v>490</v>
@@ -5302,7 +5581,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B52">
         <v>14.6</v>
@@ -5317,7 +5596,7 @@
         <v>1.15</v>
       </c>
       <c r="F52" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G52">
         <v>679</v>
@@ -5328,7 +5607,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B53">
         <v>9.06</v>
@@ -5345,7 +5624,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="B54">
         <v>18.8904</v>
@@ -5375,57 +5654,57 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B2">
         <v>0.06</v>
@@ -5452,10 +5731,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -5478,7 +5757,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B3">
         <v>0.06</v>
@@ -5505,10 +5784,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -5531,7 +5810,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B4">
         <v>0.04</v>
@@ -5558,10 +5837,10 @@
         <v>150</v>
       </c>
       <c r="J4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5584,7 +5863,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -5611,10 +5890,10 @@
         <v>150</v>
       </c>
       <c r="J5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5637,7 +5916,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <v>0.07000000000000001</v>
@@ -5664,10 +5943,10 @@
         <v>150</v>
       </c>
       <c r="J6" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -5690,7 +5969,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B7">
         <v>0.04</v>
@@ -5717,10 +5996,10 @@
         <v>150</v>
       </c>
       <c r="J7" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5743,7 +6022,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -5770,10 +6049,10 @@
         <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -5796,7 +6075,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B9">
         <v>0.07000000000000001</v>
@@ -5823,10 +6102,10 @@
         <v>150</v>
       </c>
       <c r="J9" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -5849,7 +6128,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>0.32</v>
@@ -5876,10 +6155,10 @@
         <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -5902,7 +6181,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B11">
         <v>0.3375</v>
@@ -5929,10 +6208,10 @@
         <v>150</v>
       </c>
       <c r="J11" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -5955,7 +6234,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B12">
         <v>0.2619</v>
@@ -5982,10 +6261,10 @@
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -6008,7 +6287,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B13">
         <v>0.24</v>
@@ -6035,10 +6314,10 @@
         <v>150</v>
       </c>
       <c r="J13" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -6061,7 +6340,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B14">
         <v>0.2375</v>
@@ -6088,10 +6367,10 @@
         <v>150</v>
       </c>
       <c r="J14" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -6114,7 +6393,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B15">
         <v>0.1873</v>
@@ -6141,10 +6420,10 @@
         <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -6167,7 +6446,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B16">
         <v>0.04</v>
@@ -6194,10 +6473,10 @@
         <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -6220,7 +6499,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>0.06</v>
@@ -6247,10 +6526,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L17">
         <v>0</v>

</xml_diff>